<commit_message>
Jenkins adding Lombok dependancy
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/resources/scenarioInfo.xlsx
+++ b/src/test/java/ApachePOI/resources/scenarioInfo.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="20">
   <si>
     <t>94ee31ed-788b-4ae4-9459-94125da44a11</t>
   </si>
@@ -57,6 +57,21 @@
   </si>
   <si>
     <t>e2fb4117-fbf2-4771-a9d6-6bb513a081f0</t>
+  </si>
+  <si>
+    <t>d9aa1b49-6548-445a-844d-efdbb3923b89</t>
+  </si>
+  <si>
+    <t>e83e7079-1f20-4704-a1a2-abdd28c61a7d</t>
+  </si>
+  <si>
+    <t>Create a new Country</t>
+  </si>
+  <si>
+    <t>87a72036-24c3-4ee6-a83f-9bc671e194c5</t>
+  </si>
+  <si>
+    <t>Delete a Country with parameters</t>
   </si>
 </sst>
 </file>
@@ -101,7 +116,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -204,6 +219,39 @@
         <v>2</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>